<commit_message>
correctie dubbele naam Roeselare en dubbele code Lommel
Een foute schrijfwijze in Roeselare en een niet-uniek geïdentificeerde wijk (beide in gemeente-gedragen wijken) zorgden voor dubbele unieke codes. Daarom:
- extra check op dubbels in script
- opnieuw verwerken basisdata swing voor ggw7
- opnieuw samenstellen verzamelbestanden
- opnieuw aanmaken geometrie
</commit_message>
<xml_diff>
--- a/data_voor_swing/aggregatietabellen/ggw7_gemeente.xlsx
+++ b/data_voor_swing/aggregatietabellen/ggw7_gemeente.xlsx
@@ -382,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2817"/>
+  <dimension ref="A1:B2818"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -26133,7 +26133,7 @@
     <row r="2575" spans="1:2" s="0" outlineLevel="0">
       <c r="A2575" t="inlineStr">
         <is>
-          <t>72020C</t>
+          <t>72020BAL</t>
         </is>
       </c>
       <c r="B2575" s="23">
@@ -26143,7 +26143,7 @@
     <row r="2576" spans="1:2" s="0" outlineLevel="0">
       <c r="A2576" t="inlineStr">
         <is>
-          <t>72020HE</t>
+          <t>72020C</t>
         </is>
       </c>
       <c r="B2576" s="23">
@@ -26153,7 +26153,7 @@
     <row r="2577" spans="1:2" s="0" outlineLevel="0">
       <c r="A2577" t="inlineStr">
         <is>
-          <t>72020HH</t>
+          <t>72020HE</t>
         </is>
       </c>
       <c r="B2577" s="23">
@@ -26163,7 +26163,7 @@
     <row r="2578" spans="1:2" s="0" outlineLevel="0">
       <c r="A2578" t="inlineStr">
         <is>
-          <t>72020KA</t>
+          <t>72020HH</t>
         </is>
       </c>
       <c r="B2578" s="23">
@@ -26173,7 +26173,7 @@
     <row r="2579" spans="1:2" s="0" outlineLevel="0">
       <c r="A2579" t="inlineStr">
         <is>
-          <t>72020KE</t>
+          <t>72020KA</t>
         </is>
       </c>
       <c r="B2579" s="23">
@@ -26183,7 +26183,7 @@
     <row r="2580" spans="1:2" s="0" outlineLevel="0">
       <c r="A2580" t="inlineStr">
         <is>
-          <t>72020KO</t>
+          <t>72020KE</t>
         </is>
       </c>
       <c r="B2580" s="23">
@@ -26193,7 +26193,7 @@
     <row r="2581" spans="1:2" s="0" outlineLevel="0">
       <c r="A2581" t="inlineStr">
         <is>
-          <t>72020LL</t>
+          <t>72020KO</t>
         </is>
       </c>
       <c r="B2581" s="23">
@@ -26203,7 +26203,7 @@
     <row r="2582" spans="1:2" s="0" outlineLevel="0">
       <c r="A2582" t="inlineStr">
         <is>
-          <t>72020ONB</t>
+          <t>72020LL</t>
         </is>
       </c>
       <c r="B2582" s="23">
@@ -26213,7 +26213,7 @@
     <row r="2583" spans="1:2" s="0" outlineLevel="0">
       <c r="A2583" t="inlineStr">
         <is>
-          <t>72020W</t>
+          <t>72020ONB</t>
         </is>
       </c>
       <c r="B2583" s="23">
@@ -26223,17 +26223,17 @@
     <row r="2584" spans="1:2" s="0" outlineLevel="0">
       <c r="A2584" t="inlineStr">
         <is>
-          <t>7202101</t>
+          <t>72020W</t>
         </is>
       </c>
       <c r="B2584" s="23">
-        <v>72021</v>
+        <v>72020</v>
       </c>
     </row>
     <row r="2585" spans="1:2" s="0" outlineLevel="0">
       <c r="A2585" t="inlineStr">
         <is>
-          <t>7202102</t>
+          <t>7202101</t>
         </is>
       </c>
       <c r="B2585" s="23">
@@ -26243,7 +26243,7 @@
     <row r="2586" spans="1:2" s="0" outlineLevel="0">
       <c r="A2586" t="inlineStr">
         <is>
-          <t>7202103</t>
+          <t>7202102</t>
         </is>
       </c>
       <c r="B2586" s="23">
@@ -26253,7 +26253,7 @@
     <row r="2587" spans="1:2" s="0" outlineLevel="0">
       <c r="A2587" t="inlineStr">
         <is>
-          <t>7202104</t>
+          <t>7202103</t>
         </is>
       </c>
       <c r="B2587" s="23">
@@ -26263,7 +26263,7 @@
     <row r="2588" spans="1:2" s="0" outlineLevel="0">
       <c r="A2588" t="inlineStr">
         <is>
-          <t>7202105</t>
+          <t>7202104</t>
         </is>
       </c>
       <c r="B2588" s="23">
@@ -26273,7 +26273,7 @@
     <row r="2589" spans="1:2" s="0" outlineLevel="0">
       <c r="A2589" t="inlineStr">
         <is>
-          <t>7202106</t>
+          <t>7202105</t>
         </is>
       </c>
       <c r="B2589" s="23">
@@ -26283,7 +26283,7 @@
     <row r="2590" spans="1:2" s="0" outlineLevel="0">
       <c r="A2590" t="inlineStr">
         <is>
-          <t>7202107</t>
+          <t>7202106</t>
         </is>
       </c>
       <c r="B2590" s="23">
@@ -26293,7 +26293,7 @@
     <row r="2591" spans="1:2" s="0" outlineLevel="0">
       <c r="A2591" t="inlineStr">
         <is>
-          <t>7202108</t>
+          <t>7202107</t>
         </is>
       </c>
       <c r="B2591" s="23">
@@ -26303,7 +26303,7 @@
     <row r="2592" spans="1:2" s="0" outlineLevel="0">
       <c r="A2592" t="inlineStr">
         <is>
-          <t>7202109</t>
+          <t>7202108</t>
         </is>
       </c>
       <c r="B2592" s="23">
@@ -26313,7 +26313,7 @@
     <row r="2593" spans="1:2" s="0" outlineLevel="0">
       <c r="A2593" t="inlineStr">
         <is>
-          <t>7202110</t>
+          <t>7202109</t>
         </is>
       </c>
       <c r="B2593" s="23">
@@ -26323,7 +26323,7 @@
     <row r="2594" spans="1:2" s="0" outlineLevel="0">
       <c r="A2594" t="inlineStr">
         <is>
-          <t>7202111</t>
+          <t>7202110</t>
         </is>
       </c>
       <c r="B2594" s="23">
@@ -26333,7 +26333,7 @@
     <row r="2595" spans="1:2" s="0" outlineLevel="0">
       <c r="A2595" t="inlineStr">
         <is>
-          <t>7202112</t>
+          <t>7202111</t>
         </is>
       </c>
       <c r="B2595" s="23">
@@ -26343,7 +26343,7 @@
     <row r="2596" spans="1:2" s="0" outlineLevel="0">
       <c r="A2596" t="inlineStr">
         <is>
-          <t>7202113</t>
+          <t>7202112</t>
         </is>
       </c>
       <c r="B2596" s="23">
@@ -26353,7 +26353,7 @@
     <row r="2597" spans="1:2" s="0" outlineLevel="0">
       <c r="A2597" t="inlineStr">
         <is>
-          <t>72021ZZZZ</t>
+          <t>7202113</t>
         </is>
       </c>
       <c r="B2597" s="23">
@@ -26363,17 +26363,17 @@
     <row r="2598" spans="1:2" s="0" outlineLevel="0">
       <c r="A2598" t="inlineStr">
         <is>
-          <t>7203001</t>
+          <t>72021ZZZZ</t>
         </is>
       </c>
       <c r="B2598" s="23">
-        <v>72030</v>
+        <v>72021</v>
       </c>
     </row>
     <row r="2599" spans="1:2" s="0" outlineLevel="0">
       <c r="A2599" t="inlineStr">
         <is>
-          <t>7203002</t>
+          <t>7203001</t>
         </is>
       </c>
       <c r="B2599" s="23">
@@ -26383,7 +26383,7 @@
     <row r="2600" spans="1:2" s="0" outlineLevel="0">
       <c r="A2600" t="inlineStr">
         <is>
-          <t>7203003</t>
+          <t>7203002</t>
         </is>
       </c>
       <c r="B2600" s="23">
@@ -26393,7 +26393,7 @@
     <row r="2601" spans="1:2" s="0" outlineLevel="0">
       <c r="A2601" t="inlineStr">
         <is>
-          <t>7203004</t>
+          <t>7203003</t>
         </is>
       </c>
       <c r="B2601" s="23">
@@ -26403,7 +26403,7 @@
     <row r="2602" spans="1:2" s="0" outlineLevel="0">
       <c r="A2602" t="inlineStr">
         <is>
-          <t>7203005</t>
+          <t>7203004</t>
         </is>
       </c>
       <c r="B2602" s="23">
@@ -26413,7 +26413,7 @@
     <row r="2603" spans="1:2" s="0" outlineLevel="0">
       <c r="A2603" t="inlineStr">
         <is>
-          <t>72030ZZZZ</t>
+          <t>7203005</t>
         </is>
       </c>
       <c r="B2603" s="23">
@@ -26423,17 +26423,17 @@
     <row r="2604" spans="1:2" s="0" outlineLevel="0">
       <c r="A2604" t="inlineStr">
         <is>
-          <t>7203701</t>
+          <t>72030ZZZZ</t>
         </is>
       </c>
       <c r="B2604" s="23">
-        <v>72037</v>
+        <v>72030</v>
       </c>
     </row>
     <row r="2605" spans="1:2" s="0" outlineLevel="0">
       <c r="A2605" t="inlineStr">
         <is>
-          <t>7203702</t>
+          <t>7203701</t>
         </is>
       </c>
       <c r="B2605" s="23">
@@ -26443,7 +26443,7 @@
     <row r="2606" spans="1:2" s="0" outlineLevel="0">
       <c r="A2606" t="inlineStr">
         <is>
-          <t>7203703</t>
+          <t>7203702</t>
         </is>
       </c>
       <c r="B2606" s="23">
@@ -26453,7 +26453,7 @@
     <row r="2607" spans="1:2" s="0" outlineLevel="0">
       <c r="A2607" t="inlineStr">
         <is>
-          <t>7203704</t>
+          <t>7203703</t>
         </is>
       </c>
       <c r="B2607" s="23">
@@ -26463,7 +26463,7 @@
     <row r="2608" spans="1:2" s="0" outlineLevel="0">
       <c r="A2608" t="inlineStr">
         <is>
-          <t>72037ZZZZ</t>
+          <t>7203704</t>
         </is>
       </c>
       <c r="B2608" s="23">
@@ -26473,17 +26473,17 @@
     <row r="2609" spans="1:2" s="0" outlineLevel="0">
       <c r="A2609" t="inlineStr">
         <is>
-          <t>72038A0</t>
+          <t>72037ZZZZ</t>
         </is>
       </c>
       <c r="B2609" s="23">
-        <v>72038</v>
+        <v>72037</v>
       </c>
     </row>
     <row r="2610" spans="1:2" s="0" outlineLevel="0">
       <c r="A2610" t="inlineStr">
         <is>
-          <t>72038A1</t>
+          <t>72038A0</t>
         </is>
       </c>
       <c r="B2610" s="23">
@@ -26493,7 +26493,7 @@
     <row r="2611" spans="1:2" s="0" outlineLevel="0">
       <c r="A2611" t="inlineStr">
         <is>
-          <t>72038A2</t>
+          <t>72038A1</t>
         </is>
       </c>
       <c r="B2611" s="23">
@@ -26503,7 +26503,7 @@
     <row r="2612" spans="1:2" s="0" outlineLevel="0">
       <c r="A2612" t="inlineStr">
         <is>
-          <t>72038B0</t>
+          <t>72038A2</t>
         </is>
       </c>
       <c r="B2612" s="23">
@@ -26513,7 +26513,7 @@
     <row r="2613" spans="1:2" s="0" outlineLevel="0">
       <c r="A2613" t="inlineStr">
         <is>
-          <t>72038B1</t>
+          <t>72038B0</t>
         </is>
       </c>
       <c r="B2613" s="23">
@@ -26523,7 +26523,7 @@
     <row r="2614" spans="1:2" s="0" outlineLevel="0">
       <c r="A2614" t="inlineStr">
         <is>
-          <t>72038B2</t>
+          <t>72038B1</t>
         </is>
       </c>
       <c r="B2614" s="23">
@@ -26533,7 +26533,7 @@
     <row r="2615" spans="1:2" s="0" outlineLevel="0">
       <c r="A2615" t="inlineStr">
         <is>
-          <t>72038B3</t>
+          <t>72038B2</t>
         </is>
       </c>
       <c r="B2615" s="23">
@@ -26543,7 +26543,7 @@
     <row r="2616" spans="1:2" s="0" outlineLevel="0">
       <c r="A2616" t="inlineStr">
         <is>
-          <t>72038ONB</t>
+          <t>72038B3</t>
         </is>
       </c>
       <c r="B2616" s="23">
@@ -26553,17 +26553,17 @@
     <row r="2617" spans="1:2" s="0" outlineLevel="0">
       <c r="A2617" t="inlineStr">
         <is>
-          <t>72039A0</t>
+          <t>72038ONB</t>
         </is>
       </c>
       <c r="B2617" s="23">
-        <v>72039</v>
+        <v>72038</v>
       </c>
     </row>
     <row r="2618" spans="1:2" s="0" outlineLevel="0">
       <c r="A2618" t="inlineStr">
         <is>
-          <t>72039A1</t>
+          <t>72039A0</t>
         </is>
       </c>
       <c r="B2618" s="23">
@@ -26573,7 +26573,7 @@
     <row r="2619" spans="1:2" s="0" outlineLevel="0">
       <c r="A2619" t="inlineStr">
         <is>
-          <t>72039A2</t>
+          <t>72039A1</t>
         </is>
       </c>
       <c r="B2619" s="23">
@@ -26583,7 +26583,7 @@
     <row r="2620" spans="1:2" s="0" outlineLevel="0">
       <c r="A2620" t="inlineStr">
         <is>
-          <t>72039A3</t>
+          <t>72039A2</t>
         </is>
       </c>
       <c r="B2620" s="23">
@@ -26593,7 +26593,7 @@
     <row r="2621" spans="1:2" s="0" outlineLevel="0">
       <c r="A2621" t="inlineStr">
         <is>
-          <t>72039B0</t>
+          <t>72039A3</t>
         </is>
       </c>
       <c r="B2621" s="23">
@@ -26603,7 +26603,7 @@
     <row r="2622" spans="1:2" s="0" outlineLevel="0">
       <c r="A2622" t="inlineStr">
         <is>
-          <t>72039B1</t>
+          <t>72039B0</t>
         </is>
       </c>
       <c r="B2622" s="23">
@@ -26613,7 +26613,7 @@
     <row r="2623" spans="1:2" s="0" outlineLevel="0">
       <c r="A2623" t="inlineStr">
         <is>
-          <t>72039ONB</t>
+          <t>72039B1</t>
         </is>
       </c>
       <c r="B2623" s="23">
@@ -26623,17 +26623,17 @@
     <row r="2624" spans="1:2" s="0" outlineLevel="0">
       <c r="A2624" t="inlineStr">
         <is>
-          <t>72040A0</t>
+          <t>72039ONB</t>
         </is>
       </c>
       <c r="B2624" s="23">
-        <v>72042</v>
+        <v>72039</v>
       </c>
     </row>
     <row r="2625" spans="1:2" s="0" outlineLevel="0">
       <c r="A2625" t="inlineStr">
         <is>
-          <t>72040A1</t>
+          <t>72040A0</t>
         </is>
       </c>
       <c r="B2625" s="23">
@@ -26643,7 +26643,7 @@
     <row r="2626" spans="1:2" s="0" outlineLevel="0">
       <c r="A2626" t="inlineStr">
         <is>
-          <t>72040A2</t>
+          <t>72040A1</t>
         </is>
       </c>
       <c r="B2626" s="23">
@@ -26653,7 +26653,7 @@
     <row r="2627" spans="1:2" s="0" outlineLevel="0">
       <c r="A2627" t="inlineStr">
         <is>
-          <t>72040B0</t>
+          <t>72040A2</t>
         </is>
       </c>
       <c r="B2627" s="23">
@@ -26663,7 +26663,7 @@
     <row r="2628" spans="1:2" s="0" outlineLevel="0">
       <c r="A2628" t="inlineStr">
         <is>
-          <t>72040B1</t>
+          <t>72040B0</t>
         </is>
       </c>
       <c r="B2628" s="23">
@@ -26673,7 +26673,7 @@
     <row r="2629" spans="1:2" s="0" outlineLevel="0">
       <c r="A2629" t="inlineStr">
         <is>
-          <t>72040C0</t>
+          <t>72040B1</t>
         </is>
       </c>
       <c r="B2629" s="23">
@@ -26683,7 +26683,7 @@
     <row r="2630" spans="1:2" s="0" outlineLevel="0">
       <c r="A2630" t="inlineStr">
         <is>
-          <t>72040D0</t>
+          <t>72040C0</t>
         </is>
       </c>
       <c r="B2630" s="23">
@@ -26693,7 +26693,7 @@
     <row r="2631" spans="1:2" s="0" outlineLevel="0">
       <c r="A2631" t="inlineStr">
         <is>
-          <t>72040D1</t>
+          <t>72040D0</t>
         </is>
       </c>
       <c r="B2631" s="23">
@@ -26703,7 +26703,7 @@
     <row r="2632" spans="1:2" s="0" outlineLevel="0">
       <c r="A2632" t="inlineStr">
         <is>
-          <t>72040D4</t>
+          <t>72040D1</t>
         </is>
       </c>
       <c r="B2632" s="23">
@@ -26713,7 +26713,7 @@
     <row r="2633" spans="1:2" s="0" outlineLevel="0">
       <c r="A2633" t="inlineStr">
         <is>
-          <t>72040E0</t>
+          <t>72040D4</t>
         </is>
       </c>
       <c r="B2633" s="23">
@@ -26723,17 +26723,17 @@
     <row r="2634" spans="1:2" s="0" outlineLevel="0">
       <c r="A2634" t="inlineStr">
         <is>
-          <t>72041A0</t>
+          <t>72040E0</t>
         </is>
       </c>
       <c r="B2634" s="23">
-        <v>72041</v>
+        <v>72042</v>
       </c>
     </row>
     <row r="2635" spans="1:2" s="0" outlineLevel="0">
       <c r="A2635" t="inlineStr">
         <is>
-          <t>72041A1</t>
+          <t>72041A0</t>
         </is>
       </c>
       <c r="B2635" s="23">
@@ -26743,7 +26743,7 @@
     <row r="2636" spans="1:2" s="0" outlineLevel="0">
       <c r="A2636" t="inlineStr">
         <is>
-          <t>72041B0</t>
+          <t>72041A1</t>
         </is>
       </c>
       <c r="B2636" s="23">
@@ -26753,7 +26753,7 @@
     <row r="2637" spans="1:2" s="0" outlineLevel="0">
       <c r="A2637" t="inlineStr">
         <is>
-          <t>72041B1</t>
+          <t>72041B0</t>
         </is>
       </c>
       <c r="B2637" s="23">
@@ -26763,7 +26763,7 @@
     <row r="2638" spans="1:2" s="0" outlineLevel="0">
       <c r="A2638" t="inlineStr">
         <is>
-          <t>72041B2</t>
+          <t>72041B1</t>
         </is>
       </c>
       <c r="B2638" s="23">
@@ -26773,7 +26773,7 @@
     <row r="2639" spans="1:2" s="0" outlineLevel="0">
       <c r="A2639" t="inlineStr">
         <is>
-          <t>72041C0</t>
+          <t>72041B2</t>
         </is>
       </c>
       <c r="B2639" s="23">
@@ -26783,7 +26783,7 @@
     <row r="2640" spans="1:2" s="0" outlineLevel="0">
       <c r="A2640" t="inlineStr">
         <is>
-          <t>72041C1</t>
+          <t>72041C0</t>
         </is>
       </c>
       <c r="B2640" s="23">
@@ -26793,7 +26793,7 @@
     <row r="2641" spans="1:2" s="0" outlineLevel="0">
       <c r="A2641" t="inlineStr">
         <is>
-          <t>72041D0</t>
+          <t>72041C1</t>
         </is>
       </c>
       <c r="B2641" s="23">
@@ -26803,7 +26803,7 @@
     <row r="2642" spans="1:2" s="0" outlineLevel="0">
       <c r="A2642" t="inlineStr">
         <is>
-          <t>72041D1</t>
+          <t>72041D0</t>
         </is>
       </c>
       <c r="B2642" s="23">
@@ -26813,7 +26813,7 @@
     <row r="2643" spans="1:2" s="0" outlineLevel="0">
       <c r="A2643" t="inlineStr">
         <is>
-          <t>72041E0</t>
+          <t>72041D1</t>
         </is>
       </c>
       <c r="B2643" s="23">
@@ -26823,7 +26823,7 @@
     <row r="2644" spans="1:2" s="0" outlineLevel="0">
       <c r="A2644" t="inlineStr">
         <is>
-          <t>72041E1</t>
+          <t>72041E0</t>
         </is>
       </c>
       <c r="B2644" s="23">
@@ -26833,7 +26833,7 @@
     <row r="2645" spans="1:2" s="0" outlineLevel="0">
       <c r="A2645" t="inlineStr">
         <is>
-          <t>72041E2</t>
+          <t>72041E1</t>
         </is>
       </c>
       <c r="B2645" s="23">
@@ -26843,7 +26843,7 @@
     <row r="2646" spans="1:2" s="0" outlineLevel="0">
       <c r="A2646" t="inlineStr">
         <is>
-          <t>72041ONB</t>
+          <t>72041E2</t>
         </is>
       </c>
       <c r="B2646" s="23">
@@ -26853,27 +26853,27 @@
     <row r="2647" spans="1:2" s="0" outlineLevel="0">
       <c r="A2647" t="inlineStr">
         <is>
-          <t>72042ONB</t>
+          <t>72041ONB</t>
         </is>
       </c>
       <c r="B2647" s="23">
-        <v>72042</v>
+        <v>72041</v>
       </c>
     </row>
     <row r="2648" spans="1:2" s="0" outlineLevel="0">
       <c r="A2648" t="inlineStr">
         <is>
-          <t>7204301</t>
+          <t>72042ONB</t>
         </is>
       </c>
       <c r="B2648" s="23">
-        <v>72043</v>
+        <v>72042</v>
       </c>
     </row>
     <row r="2649" spans="1:2" s="0" outlineLevel="0">
       <c r="A2649" t="inlineStr">
         <is>
-          <t>7204302</t>
+          <t>7204301</t>
         </is>
       </c>
       <c r="B2649" s="23">
@@ -26883,7 +26883,7 @@
     <row r="2650" spans="1:2" s="0" outlineLevel="0">
       <c r="A2650" t="inlineStr">
         <is>
-          <t>7204303</t>
+          <t>7204302</t>
         </is>
       </c>
       <c r="B2650" s="23">
@@ -26893,7 +26893,7 @@
     <row r="2651" spans="1:2" s="0" outlineLevel="0">
       <c r="A2651" t="inlineStr">
         <is>
-          <t>7204304</t>
+          <t>7204303</t>
         </is>
       </c>
       <c r="B2651" s="23">
@@ -26903,7 +26903,7 @@
     <row r="2652" spans="1:2" s="0" outlineLevel="0">
       <c r="A2652" t="inlineStr">
         <is>
-          <t>7204305</t>
+          <t>7204304</t>
         </is>
       </c>
       <c r="B2652" s="23">
@@ -26913,7 +26913,7 @@
     <row r="2653" spans="1:2" s="0" outlineLevel="0">
       <c r="A2653" t="inlineStr">
         <is>
-          <t>7204306</t>
+          <t>7204305</t>
         </is>
       </c>
       <c r="B2653" s="23">
@@ -26923,7 +26923,7 @@
     <row r="2654" spans="1:2" s="0" outlineLevel="0">
       <c r="A2654" t="inlineStr">
         <is>
-          <t>7204307</t>
+          <t>7204306</t>
         </is>
       </c>
       <c r="B2654" s="23">
@@ -26933,7 +26933,7 @@
     <row r="2655" spans="1:2" s="0" outlineLevel="0">
       <c r="A2655" t="inlineStr">
         <is>
-          <t>7204308</t>
+          <t>7204307</t>
         </is>
       </c>
       <c r="B2655" s="23">
@@ -26943,7 +26943,7 @@
     <row r="2656" spans="1:2" s="0" outlineLevel="0">
       <c r="A2656" t="inlineStr">
         <is>
-          <t>7204309</t>
+          <t>7204308</t>
         </is>
       </c>
       <c r="B2656" s="23">
@@ -26953,7 +26953,7 @@
     <row r="2657" spans="1:2" s="0" outlineLevel="0">
       <c r="A2657" t="inlineStr">
         <is>
-          <t>7204310</t>
+          <t>7204309</t>
         </is>
       </c>
       <c r="B2657" s="23">
@@ -26963,7 +26963,7 @@
     <row r="2658" spans="1:2" s="0" outlineLevel="0">
       <c r="A2658" t="inlineStr">
         <is>
-          <t>72043ZZZZ</t>
+          <t>7204310</t>
         </is>
       </c>
       <c r="B2658" s="23">
@@ -26973,17 +26973,17 @@
     <row r="2659" spans="1:2" s="0" outlineLevel="0">
       <c r="A2659" t="inlineStr">
         <is>
-          <t>73001A0</t>
+          <t>72043ZZZZ</t>
         </is>
       </c>
       <c r="B2659" s="23">
-        <v>73001</v>
+        <v>72043</v>
       </c>
     </row>
     <row r="2660" spans="1:2" s="0" outlineLevel="0">
       <c r="A2660" t="inlineStr">
         <is>
-          <t>73001A1</t>
+          <t>73001A0</t>
         </is>
       </c>
       <c r="B2660" s="23">
@@ -26993,7 +26993,7 @@
     <row r="2661" spans="1:2" s="0" outlineLevel="0">
       <c r="A2661" t="inlineStr">
         <is>
-          <t>73001A2</t>
+          <t>73001A1</t>
         </is>
       </c>
       <c r="B2661" s="23">
@@ -27003,7 +27003,7 @@
     <row r="2662" spans="1:2" s="0" outlineLevel="0">
       <c r="A2662" t="inlineStr">
         <is>
-          <t>73001A3</t>
+          <t>73001A2</t>
         </is>
       </c>
       <c r="B2662" s="23">
@@ -27013,7 +27013,7 @@
     <row r="2663" spans="1:2" s="0" outlineLevel="0">
       <c r="A2663" t="inlineStr">
         <is>
-          <t>73001A4</t>
+          <t>73001A3</t>
         </is>
       </c>
       <c r="B2663" s="23">
@@ -27023,7 +27023,7 @@
     <row r="2664" spans="1:2" s="0" outlineLevel="0">
       <c r="A2664" t="inlineStr">
         <is>
-          <t>73001ONB</t>
+          <t>73001A4</t>
         </is>
       </c>
       <c r="B2664" s="23">
@@ -27033,17 +27033,17 @@
     <row r="2665" spans="1:2" s="0" outlineLevel="0">
       <c r="A2665" t="inlineStr">
         <is>
-          <t>73006A0</t>
+          <t>73001ONB</t>
         </is>
       </c>
       <c r="B2665" s="23">
-        <v>73006</v>
+        <v>73001</v>
       </c>
     </row>
     <row r="2666" spans="1:2" s="0" outlineLevel="0">
       <c r="A2666" t="inlineStr">
         <is>
-          <t>73006A1</t>
+          <t>73006A0</t>
         </is>
       </c>
       <c r="B2666" s="23">
@@ -27053,7 +27053,7 @@
     <row r="2667" spans="1:2" s="0" outlineLevel="0">
       <c r="A2667" t="inlineStr">
         <is>
-          <t>73006A2</t>
+          <t>73006A1</t>
         </is>
       </c>
       <c r="B2667" s="23">
@@ -27063,7 +27063,7 @@
     <row r="2668" spans="1:2" s="0" outlineLevel="0">
       <c r="A2668" t="inlineStr">
         <is>
-          <t>73006A3</t>
+          <t>73006A2</t>
         </is>
       </c>
       <c r="B2668" s="23">
@@ -27073,7 +27073,7 @@
     <row r="2669" spans="1:2" s="0" outlineLevel="0">
       <c r="A2669" t="inlineStr">
         <is>
-          <t>73006B0</t>
+          <t>73006A3</t>
         </is>
       </c>
       <c r="B2669" s="23">
@@ -27083,7 +27083,7 @@
     <row r="2670" spans="1:2" s="0" outlineLevel="0">
       <c r="A2670" t="inlineStr">
         <is>
-          <t>73006B1</t>
+          <t>73006B0</t>
         </is>
       </c>
       <c r="B2670" s="23">
@@ -27093,7 +27093,7 @@
     <row r="2671" spans="1:2" s="0" outlineLevel="0">
       <c r="A2671" t="inlineStr">
         <is>
-          <t>73006C0</t>
+          <t>73006B1</t>
         </is>
       </c>
       <c r="B2671" s="23">
@@ -27103,7 +27103,7 @@
     <row r="2672" spans="1:2" s="0" outlineLevel="0">
       <c r="A2672" t="inlineStr">
         <is>
-          <t>73006D0</t>
+          <t>73006C0</t>
         </is>
       </c>
       <c r="B2672" s="23">
@@ -27113,7 +27113,7 @@
     <row r="2673" spans="1:2" s="0" outlineLevel="0">
       <c r="A2673" t="inlineStr">
         <is>
-          <t>73006E0</t>
+          <t>73006D0</t>
         </is>
       </c>
       <c r="B2673" s="23">
@@ -27123,7 +27123,7 @@
     <row r="2674" spans="1:2" s="0" outlineLevel="0">
       <c r="A2674" t="inlineStr">
         <is>
-          <t>73006F0</t>
+          <t>73006E0</t>
         </is>
       </c>
       <c r="B2674" s="23">
@@ -27133,7 +27133,7 @@
     <row r="2675" spans="1:2" s="0" outlineLevel="0">
       <c r="A2675" t="inlineStr">
         <is>
-          <t>73006F1</t>
+          <t>73006F0</t>
         </is>
       </c>
       <c r="B2675" s="23">
@@ -27143,7 +27143,7 @@
     <row r="2676" spans="1:2" s="0" outlineLevel="0">
       <c r="A2676" t="inlineStr">
         <is>
-          <t>73006G0</t>
+          <t>73006F1</t>
         </is>
       </c>
       <c r="B2676" s="23">
@@ -27153,7 +27153,7 @@
     <row r="2677" spans="1:2" s="0" outlineLevel="0">
       <c r="A2677" t="inlineStr">
         <is>
-          <t>73006H0</t>
+          <t>73006G0</t>
         </is>
       </c>
       <c r="B2677" s="23">
@@ -27163,7 +27163,7 @@
     <row r="2678" spans="1:2" s="0" outlineLevel="0">
       <c r="A2678" t="inlineStr">
         <is>
-          <t>73006J0</t>
+          <t>73006H0</t>
         </is>
       </c>
       <c r="B2678" s="23">
@@ -27173,7 +27173,7 @@
     <row r="2679" spans="1:2" s="0" outlineLevel="0">
       <c r="A2679" t="inlineStr">
         <is>
-          <t>73006K0</t>
+          <t>73006J0</t>
         </is>
       </c>
       <c r="B2679" s="23">
@@ -27183,7 +27183,7 @@
     <row r="2680" spans="1:2" s="0" outlineLevel="0">
       <c r="A2680" t="inlineStr">
         <is>
-          <t>73006L0</t>
+          <t>73006K0</t>
         </is>
       </c>
       <c r="B2680" s="23">
@@ -27193,7 +27193,7 @@
     <row r="2681" spans="1:2" s="0" outlineLevel="0">
       <c r="A2681" t="inlineStr">
         <is>
-          <t>73006M0</t>
+          <t>73006L0</t>
         </is>
       </c>
       <c r="B2681" s="23">
@@ -27203,7 +27203,7 @@
     <row r="2682" spans="1:2" s="0" outlineLevel="0">
       <c r="A2682" t="inlineStr">
         <is>
-          <t>73006M1</t>
+          <t>73006M0</t>
         </is>
       </c>
       <c r="B2682" s="23">
@@ -27213,7 +27213,7 @@
     <row r="2683" spans="1:2" s="0" outlineLevel="0">
       <c r="A2683" t="inlineStr">
         <is>
-          <t>73006N0</t>
+          <t>73006M1</t>
         </is>
       </c>
       <c r="B2683" s="23">
@@ -27223,7 +27223,7 @@
     <row r="2684" spans="1:2" s="0" outlineLevel="0">
       <c r="A2684" t="inlineStr">
         <is>
-          <t>73006ONB</t>
+          <t>73006N0</t>
         </is>
       </c>
       <c r="B2684" s="23">
@@ -27233,17 +27233,17 @@
     <row r="2685" spans="1:2" s="0" outlineLevel="0">
       <c r="A2685" t="inlineStr">
         <is>
-          <t>73009A0</t>
+          <t>73006ONB</t>
         </is>
       </c>
       <c r="B2685" s="23">
-        <v>73009</v>
+        <v>73006</v>
       </c>
     </row>
     <row r="2686" spans="1:2" s="0" outlineLevel="0">
       <c r="A2686" t="inlineStr">
         <is>
-          <t>73009B0</t>
+          <t>73009A0</t>
         </is>
       </c>
       <c r="B2686" s="23">
@@ -27253,7 +27253,7 @@
     <row r="2687" spans="1:2" s="0" outlineLevel="0">
       <c r="A2687" t="inlineStr">
         <is>
-          <t>73009C0</t>
+          <t>73009B0</t>
         </is>
       </c>
       <c r="B2687" s="23">
@@ -27263,7 +27263,7 @@
     <row r="2688" spans="1:2" s="0" outlineLevel="0">
       <c r="A2688" t="inlineStr">
         <is>
-          <t>73009D0</t>
+          <t>73009C0</t>
         </is>
       </c>
       <c r="B2688" s="23">
@@ -27273,7 +27273,7 @@
     <row r="2689" spans="1:2" s="0" outlineLevel="0">
       <c r="A2689" t="inlineStr">
         <is>
-          <t>73009E0</t>
+          <t>73009D0</t>
         </is>
       </c>
       <c r="B2689" s="23">
@@ -27283,7 +27283,7 @@
     <row r="2690" spans="1:2" s="0" outlineLevel="0">
       <c r="A2690" t="inlineStr">
         <is>
-          <t>73009F0</t>
+          <t>73009E0</t>
         </is>
       </c>
       <c r="B2690" s="23">
@@ -27293,7 +27293,7 @@
     <row r="2691" spans="1:2" s="0" outlineLevel="0">
       <c r="A2691" t="inlineStr">
         <is>
-          <t>73009G0</t>
+          <t>73009F0</t>
         </is>
       </c>
       <c r="B2691" s="23">
@@ -27303,7 +27303,7 @@
     <row r="2692" spans="1:2" s="0" outlineLevel="0">
       <c r="A2692" t="inlineStr">
         <is>
-          <t>73009H0</t>
+          <t>73009G0</t>
         </is>
       </c>
       <c r="B2692" s="23">
@@ -27313,7 +27313,7 @@
     <row r="2693" spans="1:2" s="0" outlineLevel="0">
       <c r="A2693" t="inlineStr">
         <is>
-          <t>73009J0</t>
+          <t>73009H0</t>
         </is>
       </c>
       <c r="B2693" s="23">
@@ -27323,7 +27323,7 @@
     <row r="2694" spans="1:2" s="0" outlineLevel="0">
       <c r="A2694" t="inlineStr">
         <is>
-          <t>73009K0</t>
+          <t>73009J0</t>
         </is>
       </c>
       <c r="B2694" s="23">
@@ -27333,7 +27333,7 @@
     <row r="2695" spans="1:2" s="0" outlineLevel="0">
       <c r="A2695" t="inlineStr">
         <is>
-          <t>73009L0</t>
+          <t>73009K0</t>
         </is>
       </c>
       <c r="B2695" s="23">
@@ -27343,7 +27343,7 @@
     <row r="2696" spans="1:2" s="0" outlineLevel="0">
       <c r="A2696" t="inlineStr">
         <is>
-          <t>73009M0</t>
+          <t>73009L0</t>
         </is>
       </c>
       <c r="B2696" s="23">
@@ -27353,7 +27353,7 @@
     <row r="2697" spans="1:2" s="0" outlineLevel="0">
       <c r="A2697" t="inlineStr">
         <is>
-          <t>73009N0</t>
+          <t>73009M0</t>
         </is>
       </c>
       <c r="B2697" s="23">
@@ -27363,7 +27363,7 @@
     <row r="2698" spans="1:2" s="0" outlineLevel="0">
       <c r="A2698" t="inlineStr">
         <is>
-          <t>73009ONB</t>
+          <t>73009N0</t>
         </is>
       </c>
       <c r="B2698" s="23">
@@ -27373,17 +27373,17 @@
     <row r="2699" spans="1:2" s="0" outlineLevel="0">
       <c r="A2699" t="inlineStr">
         <is>
-          <t>73022A0</t>
+          <t>73009ONB</t>
         </is>
       </c>
       <c r="B2699" s="23">
-        <v>73022</v>
+        <v>73009</v>
       </c>
     </row>
     <row r="2700" spans="1:2" s="0" outlineLevel="0">
       <c r="A2700" t="inlineStr">
         <is>
-          <t>73022B0</t>
+          <t>73022A0</t>
         </is>
       </c>
       <c r="B2700" s="23">
@@ -27393,7 +27393,7 @@
     <row r="2701" spans="1:2" s="0" outlineLevel="0">
       <c r="A2701" t="inlineStr">
         <is>
-          <t>73022C0</t>
+          <t>73022B0</t>
         </is>
       </c>
       <c r="B2701" s="23">
@@ -27403,7 +27403,7 @@
     <row r="2702" spans="1:2" s="0" outlineLevel="0">
       <c r="A2702" t="inlineStr">
         <is>
-          <t>73022D0</t>
+          <t>73022C0</t>
         </is>
       </c>
       <c r="B2702" s="23">
@@ -27413,7 +27413,7 @@
     <row r="2703" spans="1:2" s="0" outlineLevel="0">
       <c r="A2703" t="inlineStr">
         <is>
-          <t>73022E0</t>
+          <t>73022D0</t>
         </is>
       </c>
       <c r="B2703" s="23">
@@ -27423,7 +27423,7 @@
     <row r="2704" spans="1:2" s="0" outlineLevel="0">
       <c r="A2704" t="inlineStr">
         <is>
-          <t>73022F0</t>
+          <t>73022E0</t>
         </is>
       </c>
       <c r="B2704" s="23">
@@ -27433,7 +27433,7 @@
     <row r="2705" spans="1:2" s="0" outlineLevel="0">
       <c r="A2705" t="inlineStr">
         <is>
-          <t>73022G0</t>
+          <t>73022F0</t>
         </is>
       </c>
       <c r="B2705" s="23">
@@ -27443,7 +27443,7 @@
     <row r="2706" spans="1:2" s="0" outlineLevel="0">
       <c r="A2706" t="inlineStr">
         <is>
-          <t>73022H0</t>
+          <t>73022G0</t>
         </is>
       </c>
       <c r="B2706" s="23">
@@ -27453,7 +27453,7 @@
     <row r="2707" spans="1:2" s="0" outlineLevel="0">
       <c r="A2707" t="inlineStr">
         <is>
-          <t>73022J0</t>
+          <t>73022H0</t>
         </is>
       </c>
       <c r="B2707" s="23">
@@ -27463,7 +27463,7 @@
     <row r="2708" spans="1:2" s="0" outlineLevel="0">
       <c r="A2708" t="inlineStr">
         <is>
-          <t>73022K0</t>
+          <t>73022J0</t>
         </is>
       </c>
       <c r="B2708" s="23">
@@ -27473,7 +27473,7 @@
     <row r="2709" spans="1:2" s="0" outlineLevel="0">
       <c r="A2709" t="inlineStr">
         <is>
-          <t>73022L0</t>
+          <t>73022K0</t>
         </is>
       </c>
       <c r="B2709" s="23">
@@ -27483,7 +27483,7 @@
     <row r="2710" spans="1:2" s="0" outlineLevel="0">
       <c r="A2710" t="inlineStr">
         <is>
-          <t>73022M0</t>
+          <t>73022L0</t>
         </is>
       </c>
       <c r="B2710" s="23">
@@ -27493,7 +27493,7 @@
     <row r="2711" spans="1:2" s="0" outlineLevel="0">
       <c r="A2711" t="inlineStr">
         <is>
-          <t>73022ONB</t>
+          <t>73022M0</t>
         </is>
       </c>
       <c r="B2711" s="23">
@@ -27503,27 +27503,27 @@
     <row r="2712" spans="1:2" s="0" outlineLevel="0">
       <c r="A2712" t="inlineStr">
         <is>
-          <t>73028A0</t>
+          <t>73022ONB</t>
         </is>
       </c>
       <c r="B2712" s="23">
-        <v>73028</v>
+        <v>73022</v>
       </c>
     </row>
     <row r="2713" spans="1:2" s="0" outlineLevel="0">
       <c r="A2713" t="inlineStr">
         <is>
-          <t>73032A0</t>
+          <t>73028A0</t>
         </is>
       </c>
       <c r="B2713" s="23">
-        <v>73032</v>
+        <v>73028</v>
       </c>
     </row>
     <row r="2714" spans="1:2" s="0" outlineLevel="0">
       <c r="A2714" t="inlineStr">
         <is>
-          <t>73032A1</t>
+          <t>73032A0</t>
         </is>
       </c>
       <c r="B2714" s="23">
@@ -27533,7 +27533,7 @@
     <row r="2715" spans="1:2" s="0" outlineLevel="0">
       <c r="A2715" t="inlineStr">
         <is>
-          <t>73032A2</t>
+          <t>73032A1</t>
         </is>
       </c>
       <c r="B2715" s="23">
@@ -27543,7 +27543,7 @@
     <row r="2716" spans="1:2" s="0" outlineLevel="0">
       <c r="A2716" t="inlineStr">
         <is>
-          <t>73032A3</t>
+          <t>73032A2</t>
         </is>
       </c>
       <c r="B2716" s="23">
@@ -27553,7 +27553,7 @@
     <row r="2717" spans="1:2" s="0" outlineLevel="0">
       <c r="A2717" t="inlineStr">
         <is>
-          <t>73032B0</t>
+          <t>73032A3</t>
         </is>
       </c>
       <c r="B2717" s="23">
@@ -27563,7 +27563,7 @@
     <row r="2718" spans="1:2" s="0" outlineLevel="0">
       <c r="A2718" t="inlineStr">
         <is>
-          <t>73032C0</t>
+          <t>73032B0</t>
         </is>
       </c>
       <c r="B2718" s="23">
@@ -27573,7 +27573,7 @@
     <row r="2719" spans="1:2" s="0" outlineLevel="0">
       <c r="A2719" t="inlineStr">
         <is>
-          <t>73032D0</t>
+          <t>73032C0</t>
         </is>
       </c>
       <c r="B2719" s="23">
@@ -27583,7 +27583,7 @@
     <row r="2720" spans="1:2" s="0" outlineLevel="0">
       <c r="A2720" t="inlineStr">
         <is>
-          <t>73032D1</t>
+          <t>73032D0</t>
         </is>
       </c>
       <c r="B2720" s="23">
@@ -27593,7 +27593,7 @@
     <row r="2721" spans="1:2" s="0" outlineLevel="0">
       <c r="A2721" t="inlineStr">
         <is>
-          <t>73032E0</t>
+          <t>73032D1</t>
         </is>
       </c>
       <c r="B2721" s="23">
@@ -27603,7 +27603,7 @@
     <row r="2722" spans="1:2" s="0" outlineLevel="0">
       <c r="A2722" t="inlineStr">
         <is>
-          <t>73032ONB</t>
+          <t>73032E0</t>
         </is>
       </c>
       <c r="B2722" s="23">
@@ -27613,17 +27613,17 @@
     <row r="2723" spans="1:2" s="0" outlineLevel="0">
       <c r="A2723" t="inlineStr">
         <is>
-          <t>73040GU</t>
+          <t>73032ONB</t>
         </is>
       </c>
       <c r="B2723" s="23">
-        <v>73040</v>
+        <v>73032</v>
       </c>
     </row>
     <row r="2724" spans="1:2" s="0" outlineLevel="0">
       <c r="A2724" t="inlineStr">
         <is>
-          <t>73040KO</t>
+          <t>73040GU</t>
         </is>
       </c>
       <c r="B2724" s="23">
@@ -27633,7 +27633,7 @@
     <row r="2725" spans="1:2" s="0" outlineLevel="0">
       <c r="A2725" t="inlineStr">
         <is>
-          <t>73040ONB</t>
+          <t>73040KO</t>
         </is>
       </c>
       <c r="B2725" s="23">
@@ -27643,7 +27643,7 @@
     <row r="2726" spans="1:2" s="0" outlineLevel="0">
       <c r="A2726" t="inlineStr">
         <is>
-          <t>73040VL</t>
+          <t>73040ONB</t>
         </is>
       </c>
       <c r="B2726" s="23">
@@ -27653,7 +27653,7 @@
     <row r="2727" spans="1:2" s="0" outlineLevel="0">
       <c r="A2727" t="inlineStr">
         <is>
-          <t>73040VR</t>
+          <t>73040VL</t>
         </is>
       </c>
       <c r="B2727" s="23">
@@ -27663,7 +27663,7 @@
     <row r="2728" spans="1:2" s="0" outlineLevel="0">
       <c r="A2728" t="inlineStr">
         <is>
-          <t>73040WI</t>
+          <t>73040VR</t>
         </is>
       </c>
       <c r="B2728" s="23">
@@ -27673,17 +27673,17 @@
     <row r="2729" spans="1:2" s="0" outlineLevel="0">
       <c r="A2729" t="inlineStr">
         <is>
-          <t>73042A0</t>
+          <t>73040WI</t>
         </is>
       </c>
       <c r="B2729" s="23">
-        <v>73042</v>
+        <v>73040</v>
       </c>
     </row>
     <row r="2730" spans="1:2" s="0" outlineLevel="0">
       <c r="A2730" t="inlineStr">
         <is>
-          <t>73042A1</t>
+          <t>73042A0</t>
         </is>
       </c>
       <c r="B2730" s="23">
@@ -27693,7 +27693,7 @@
     <row r="2731" spans="1:2" s="0" outlineLevel="0">
       <c r="A2731" t="inlineStr">
         <is>
-          <t>73042A2</t>
+          <t>73042A1</t>
         </is>
       </c>
       <c r="B2731" s="23">
@@ -27703,7 +27703,7 @@
     <row r="2732" spans="1:2" s="0" outlineLevel="0">
       <c r="A2732" t="inlineStr">
         <is>
-          <t>73042A3</t>
+          <t>73042A2</t>
         </is>
       </c>
       <c r="B2732" s="23">
@@ -27713,7 +27713,7 @@
     <row r="2733" spans="1:2" s="0" outlineLevel="0">
       <c r="A2733" t="inlineStr">
         <is>
-          <t>73042A4</t>
+          <t>73042A3</t>
         </is>
       </c>
       <c r="B2733" s="23">
@@ -27723,7 +27723,7 @@
     <row r="2734" spans="1:2" s="0" outlineLevel="0">
       <c r="A2734" t="inlineStr">
         <is>
-          <t>73042A5</t>
+          <t>73042A4</t>
         </is>
       </c>
       <c r="B2734" s="23">
@@ -27733,7 +27733,7 @@
     <row r="2735" spans="1:2" s="0" outlineLevel="0">
       <c r="A2735" t="inlineStr">
         <is>
-          <t>73042B0</t>
+          <t>73042A5</t>
         </is>
       </c>
       <c r="B2735" s="23">
@@ -27743,7 +27743,7 @@
     <row r="2736" spans="1:2" s="0" outlineLevel="0">
       <c r="A2736" t="inlineStr">
         <is>
-          <t>73042B1</t>
+          <t>73042B0</t>
         </is>
       </c>
       <c r="B2736" s="23">
@@ -27753,7 +27753,7 @@
     <row r="2737" spans="1:2" s="0" outlineLevel="0">
       <c r="A2737" t="inlineStr">
         <is>
-          <t>73042C0</t>
+          <t>73042B1</t>
         </is>
       </c>
       <c r="B2737" s="23">
@@ -27763,7 +27763,7 @@
     <row r="2738" spans="1:2" s="0" outlineLevel="0">
       <c r="A2738" t="inlineStr">
         <is>
-          <t>73042D0</t>
+          <t>73042C0</t>
         </is>
       </c>
       <c r="B2738" s="23">
@@ -27773,7 +27773,7 @@
     <row r="2739" spans="1:2" s="0" outlineLevel="0">
       <c r="A2739" t="inlineStr">
         <is>
-          <t>73042D1</t>
+          <t>73042D0</t>
         </is>
       </c>
       <c r="B2739" s="23">
@@ -27783,7 +27783,7 @@
     <row r="2740" spans="1:2" s="0" outlineLevel="0">
       <c r="A2740" t="inlineStr">
         <is>
-          <t>73042E0</t>
+          <t>73042D1</t>
         </is>
       </c>
       <c r="B2740" s="23">
@@ -27793,7 +27793,7 @@
     <row r="2741" spans="1:2" s="0" outlineLevel="0">
       <c r="A2741" t="inlineStr">
         <is>
-          <t>73042E1</t>
+          <t>73042E0</t>
         </is>
       </c>
       <c r="B2741" s="23">
@@ -27803,7 +27803,7 @@
     <row r="2742" spans="1:2" s="0" outlineLevel="0">
       <c r="A2742" t="inlineStr">
         <is>
-          <t>73042ONB</t>
+          <t>73042E1</t>
         </is>
       </c>
       <c r="B2742" s="23">
@@ -27813,17 +27813,17 @@
     <row r="2743" spans="1:2" s="0" outlineLevel="0">
       <c r="A2743" t="inlineStr">
         <is>
-          <t>73066A0</t>
+          <t>73042ONB</t>
         </is>
       </c>
       <c r="B2743" s="23">
-        <v>73066</v>
+        <v>73042</v>
       </c>
     </row>
     <row r="2744" spans="1:2" s="0" outlineLevel="0">
       <c r="A2744" t="inlineStr">
         <is>
-          <t>73066B0</t>
+          <t>73066A0</t>
         </is>
       </c>
       <c r="B2744" s="23">
@@ -27833,7 +27833,7 @@
     <row r="2745" spans="1:2" s="0" outlineLevel="0">
       <c r="A2745" t="inlineStr">
         <is>
-          <t>73066C0</t>
+          <t>73066B0</t>
         </is>
       </c>
       <c r="B2745" s="23">
@@ -27843,7 +27843,7 @@
     <row r="2746" spans="1:2" s="0" outlineLevel="0">
       <c r="A2746" t="inlineStr">
         <is>
-          <t>73066D0</t>
+          <t>73066C0</t>
         </is>
       </c>
       <c r="B2746" s="23">
@@ -27853,7 +27853,7 @@
     <row r="2747" spans="1:2" s="0" outlineLevel="0">
       <c r="A2747" t="inlineStr">
         <is>
-          <t>73066E0</t>
+          <t>73066D0</t>
         </is>
       </c>
       <c r="B2747" s="23">
@@ -27863,7 +27863,7 @@
     <row r="2748" spans="1:2" s="0" outlineLevel="0">
       <c r="A2748" t="inlineStr">
         <is>
-          <t>73066F0</t>
+          <t>73066E0</t>
         </is>
       </c>
       <c r="B2748" s="23">
@@ -27873,7 +27873,7 @@
     <row r="2749" spans="1:2" s="0" outlineLevel="0">
       <c r="A2749" t="inlineStr">
         <is>
-          <t>73066F1</t>
+          <t>73066F0</t>
         </is>
       </c>
       <c r="B2749" s="23">
@@ -27883,7 +27883,7 @@
     <row r="2750" spans="1:2" s="0" outlineLevel="0">
       <c r="A2750" t="inlineStr">
         <is>
-          <t>73066G0</t>
+          <t>73066F1</t>
         </is>
       </c>
       <c r="B2750" s="23">
@@ -27893,7 +27893,7 @@
     <row r="2751" spans="1:2" s="0" outlineLevel="0">
       <c r="A2751" t="inlineStr">
         <is>
-          <t>73066G1</t>
+          <t>73066G0</t>
         </is>
       </c>
       <c r="B2751" s="23">
@@ -27903,7 +27903,7 @@
     <row r="2752" spans="1:2" s="0" outlineLevel="0">
       <c r="A2752" t="inlineStr">
         <is>
-          <t>73066H0</t>
+          <t>73066G1</t>
         </is>
       </c>
       <c r="B2752" s="23">
@@ -27913,7 +27913,7 @@
     <row r="2753" spans="1:2" s="0" outlineLevel="0">
       <c r="A2753" t="inlineStr">
         <is>
-          <t>73066J0</t>
+          <t>73066H0</t>
         </is>
       </c>
       <c r="B2753" s="23">
@@ -27923,7 +27923,7 @@
     <row r="2754" spans="1:2" s="0" outlineLevel="0">
       <c r="A2754" t="inlineStr">
         <is>
-          <t>73066K0</t>
+          <t>73066J0</t>
         </is>
       </c>
       <c r="B2754" s="23">
@@ -27933,7 +27933,7 @@
     <row r="2755" spans="1:2" s="0" outlineLevel="0">
       <c r="A2755" t="inlineStr">
         <is>
-          <t>73066ONB</t>
+          <t>73066K0</t>
         </is>
       </c>
       <c r="B2755" s="23">
@@ -27943,17 +27943,17 @@
     <row r="2756" spans="1:2" s="0" outlineLevel="0">
       <c r="A2756" t="inlineStr">
         <is>
-          <t>73083A0</t>
+          <t>73066ONB</t>
         </is>
       </c>
       <c r="B2756" s="23">
-        <v>73083</v>
+        <v>73066</v>
       </c>
     </row>
     <row r="2757" spans="1:2" s="0" outlineLevel="0">
       <c r="A2757" t="inlineStr">
         <is>
-          <t>73083A1</t>
+          <t>73083A0</t>
         </is>
       </c>
       <c r="B2757" s="23">
@@ -27963,7 +27963,7 @@
     <row r="2758" spans="1:2" s="0" outlineLevel="0">
       <c r="A2758" t="inlineStr">
         <is>
-          <t>73083A2</t>
+          <t>73083A1</t>
         </is>
       </c>
       <c r="B2758" s="23">
@@ -27973,7 +27973,7 @@
     <row r="2759" spans="1:2" s="0" outlineLevel="0">
       <c r="A2759" t="inlineStr">
         <is>
-          <t>73083A3</t>
+          <t>73083A2</t>
         </is>
       </c>
       <c r="B2759" s="23">
@@ -27983,7 +27983,7 @@
     <row r="2760" spans="1:2" s="0" outlineLevel="0">
       <c r="A2760" t="inlineStr">
         <is>
-          <t>73083A4</t>
+          <t>73083A3</t>
         </is>
       </c>
       <c r="B2760" s="23">
@@ -27993,7 +27993,7 @@
     <row r="2761" spans="1:2" s="0" outlineLevel="0">
       <c r="A2761" t="inlineStr">
         <is>
-          <t>73083A5</t>
+          <t>73083A4</t>
         </is>
       </c>
       <c r="B2761" s="23">
@@ -28003,7 +28003,7 @@
     <row r="2762" spans="1:2" s="0" outlineLevel="0">
       <c r="A2762" t="inlineStr">
         <is>
-          <t>73083B0</t>
+          <t>73083A5</t>
         </is>
       </c>
       <c r="B2762" s="23">
@@ -28013,7 +28013,7 @@
     <row r="2763" spans="1:2" s="0" outlineLevel="0">
       <c r="A2763" t="inlineStr">
         <is>
-          <t>73083C0</t>
+          <t>73083B0</t>
         </is>
       </c>
       <c r="B2763" s="23">
@@ -28023,7 +28023,7 @@
     <row r="2764" spans="1:2" s="0" outlineLevel="0">
       <c r="A2764" t="inlineStr">
         <is>
-          <t>73083D0</t>
+          <t>73083C0</t>
         </is>
       </c>
       <c r="B2764" s="23">
@@ -28033,7 +28033,7 @@
     <row r="2765" spans="1:2" s="0" outlineLevel="0">
       <c r="A2765" t="inlineStr">
         <is>
-          <t>73083D1</t>
+          <t>73083D0</t>
         </is>
       </c>
       <c r="B2765" s="23">
@@ -28043,7 +28043,7 @@
     <row r="2766" spans="1:2" s="0" outlineLevel="0">
       <c r="A2766" t="inlineStr">
         <is>
-          <t>73083E0</t>
+          <t>73083D1</t>
         </is>
       </c>
       <c r="B2766" s="23">
@@ -28053,7 +28053,7 @@
     <row r="2767" spans="1:2" s="0" outlineLevel="0">
       <c r="A2767" t="inlineStr">
         <is>
-          <t>73083E1</t>
+          <t>73083E0</t>
         </is>
       </c>
       <c r="B2767" s="23">
@@ -28063,7 +28063,7 @@
     <row r="2768" spans="1:2" s="0" outlineLevel="0">
       <c r="A2768" t="inlineStr">
         <is>
-          <t>73083F0</t>
+          <t>73083E1</t>
         </is>
       </c>
       <c r="B2768" s="23">
@@ -28073,7 +28073,7 @@
     <row r="2769" spans="1:2" s="0" outlineLevel="0">
       <c r="A2769" t="inlineStr">
         <is>
-          <t>73083G0</t>
+          <t>73083F0</t>
         </is>
       </c>
       <c r="B2769" s="23">
@@ -28083,7 +28083,7 @@
     <row r="2770" spans="1:2" s="0" outlineLevel="0">
       <c r="A2770" t="inlineStr">
         <is>
-          <t>73083G1</t>
+          <t>73083G0</t>
         </is>
       </c>
       <c r="B2770" s="23">
@@ -28093,7 +28093,7 @@
     <row r="2771" spans="1:2" s="0" outlineLevel="0">
       <c r="A2771" t="inlineStr">
         <is>
-          <t>73083H0</t>
+          <t>73083G1</t>
         </is>
       </c>
       <c r="B2771" s="23">
@@ -28103,7 +28103,7 @@
     <row r="2772" spans="1:2" s="0" outlineLevel="0">
       <c r="A2772" t="inlineStr">
         <is>
-          <t>73083J0</t>
+          <t>73083H0</t>
         </is>
       </c>
       <c r="B2772" s="23">
@@ -28113,7 +28113,7 @@
     <row r="2773" spans="1:2" s="0" outlineLevel="0">
       <c r="A2773" t="inlineStr">
         <is>
-          <t>73083K0</t>
+          <t>73083J0</t>
         </is>
       </c>
       <c r="B2773" s="23">
@@ -28123,7 +28123,7 @@
     <row r="2774" spans="1:2" s="0" outlineLevel="0">
       <c r="A2774" t="inlineStr">
         <is>
-          <t>73083K1</t>
+          <t>73083K0</t>
         </is>
       </c>
       <c r="B2774" s="23">
@@ -28133,7 +28133,7 @@
     <row r="2775" spans="1:2" s="0" outlineLevel="0">
       <c r="A2775" t="inlineStr">
         <is>
-          <t>73083L0</t>
+          <t>73083K1</t>
         </is>
       </c>
       <c r="B2775" s="23">
@@ -28143,7 +28143,7 @@
     <row r="2776" spans="1:2" s="0" outlineLevel="0">
       <c r="A2776" t="inlineStr">
         <is>
-          <t>73083M0</t>
+          <t>73083L0</t>
         </is>
       </c>
       <c r="B2776" s="23">
@@ -28153,7 +28153,7 @@
     <row r="2777" spans="1:2" s="0" outlineLevel="0">
       <c r="A2777" t="inlineStr">
         <is>
-          <t>73083N0</t>
+          <t>73083M0</t>
         </is>
       </c>
       <c r="B2777" s="23">
@@ -28163,7 +28163,7 @@
     <row r="2778" spans="1:2" s="0" outlineLevel="0">
       <c r="A2778" t="inlineStr">
         <is>
-          <t>73083ONB</t>
+          <t>73083N0</t>
         </is>
       </c>
       <c r="B2778" s="23">
@@ -28173,7 +28173,7 @@
     <row r="2779" spans="1:2" s="0" outlineLevel="0">
       <c r="A2779" t="inlineStr">
         <is>
-          <t>73083P0</t>
+          <t>73083ONB</t>
         </is>
       </c>
       <c r="B2779" s="23">
@@ -28183,7 +28183,7 @@
     <row r="2780" spans="1:2" s="0" outlineLevel="0">
       <c r="A2780" t="inlineStr">
         <is>
-          <t>73083R0</t>
+          <t>73083P0</t>
         </is>
       </c>
       <c r="B2780" s="23">
@@ -28193,7 +28193,7 @@
     <row r="2781" spans="1:2" s="0" outlineLevel="0">
       <c r="A2781" t="inlineStr">
         <is>
-          <t>73083S0</t>
+          <t>73083R0</t>
         </is>
       </c>
       <c r="B2781" s="23">
@@ -28203,17 +28203,17 @@
     <row r="2782" spans="1:2" s="0" outlineLevel="0">
       <c r="A2782" t="inlineStr">
         <is>
-          <t>73098A0</t>
+          <t>73083S0</t>
         </is>
       </c>
       <c r="B2782" s="23">
-        <v>73098</v>
+        <v>73083</v>
       </c>
     </row>
     <row r="2783" spans="1:2" s="0" outlineLevel="0">
       <c r="A2783" t="inlineStr">
         <is>
-          <t>73098A1</t>
+          <t>73098A0</t>
         </is>
       </c>
       <c r="B2783" s="23">
@@ -28223,7 +28223,7 @@
     <row r="2784" spans="1:2" s="0" outlineLevel="0">
       <c r="A2784" t="inlineStr">
         <is>
-          <t>73098A2</t>
+          <t>73098A1</t>
         </is>
       </c>
       <c r="B2784" s="23">
@@ -28233,7 +28233,7 @@
     <row r="2785" spans="1:2" s="0" outlineLevel="0">
       <c r="A2785" t="inlineStr">
         <is>
-          <t>73098A3</t>
+          <t>73098A2</t>
         </is>
       </c>
       <c r="B2785" s="23">
@@ -28243,7 +28243,7 @@
     <row r="2786" spans="1:2" s="0" outlineLevel="0">
       <c r="A2786" t="inlineStr">
         <is>
-          <t>73098B0</t>
+          <t>73098A3</t>
         </is>
       </c>
       <c r="B2786" s="23">
@@ -28253,7 +28253,7 @@
     <row r="2787" spans="1:2" s="0" outlineLevel="0">
       <c r="A2787" t="inlineStr">
         <is>
-          <t>73098C0</t>
+          <t>73098B0</t>
         </is>
       </c>
       <c r="B2787" s="23">
@@ -28263,7 +28263,7 @@
     <row r="2788" spans="1:2" s="0" outlineLevel="0">
       <c r="A2788" t="inlineStr">
         <is>
-          <t>73098D0</t>
+          <t>73098C0</t>
         </is>
       </c>
       <c r="B2788" s="23">
@@ -28273,7 +28273,7 @@
     <row r="2789" spans="1:2" s="0" outlineLevel="0">
       <c r="A2789" t="inlineStr">
         <is>
-          <t>73098ONB</t>
+          <t>73098D0</t>
         </is>
       </c>
       <c r="B2789" s="23">
@@ -28283,17 +28283,17 @@
     <row r="2790" spans="1:2" s="0" outlineLevel="0">
       <c r="A2790" t="inlineStr">
         <is>
-          <t>7310710A</t>
+          <t>73098ONB</t>
         </is>
       </c>
       <c r="B2790" s="23">
-        <v>73107</v>
+        <v>73098</v>
       </c>
     </row>
     <row r="2791" spans="1:2" s="0" outlineLevel="0">
       <c r="A2791" t="inlineStr">
         <is>
-          <t>7310710B</t>
+          <t>7310710A</t>
         </is>
       </c>
       <c r="B2791" s="23">
@@ -28303,7 +28303,7 @@
     <row r="2792" spans="1:2" s="0" outlineLevel="0">
       <c r="A2792" t="inlineStr">
         <is>
-          <t>7310711</t>
+          <t>7310710B</t>
         </is>
       </c>
       <c r="B2792" s="23">
@@ -28313,7 +28313,7 @@
     <row r="2793" spans="1:2" s="0" outlineLevel="0">
       <c r="A2793" t="inlineStr">
         <is>
-          <t>7310713</t>
+          <t>7310711</t>
         </is>
       </c>
       <c r="B2793" s="23">
@@ -28323,7 +28323,7 @@
     <row r="2794" spans="1:2" s="0" outlineLevel="0">
       <c r="A2794" t="inlineStr">
         <is>
-          <t>7310714</t>
+          <t>7310713</t>
         </is>
       </c>
       <c r="B2794" s="23">
@@ -28333,7 +28333,7 @@
     <row r="2795" spans="1:2" s="0" outlineLevel="0">
       <c r="A2795" t="inlineStr">
         <is>
-          <t>7310715</t>
+          <t>7310714</t>
         </is>
       </c>
       <c r="B2795" s="23">
@@ -28343,7 +28343,7 @@
     <row r="2796" spans="1:2" s="0" outlineLevel="0">
       <c r="A2796" t="inlineStr">
         <is>
-          <t>7310716</t>
+          <t>7310715</t>
         </is>
       </c>
       <c r="B2796" s="23">
@@ -28353,7 +28353,7 @@
     <row r="2797" spans="1:2" s="0" outlineLevel="0">
       <c r="A2797" t="inlineStr">
         <is>
-          <t>7310717</t>
+          <t>7310716</t>
         </is>
       </c>
       <c r="B2797" s="23">
@@ -28363,7 +28363,7 @@
     <row r="2798" spans="1:2" s="0" outlineLevel="0">
       <c r="A2798" t="inlineStr">
         <is>
-          <t>7310720</t>
+          <t>7310717</t>
         </is>
       </c>
       <c r="B2798" s="23">
@@ -28373,7 +28373,7 @@
     <row r="2799" spans="1:2" s="0" outlineLevel="0">
       <c r="A2799" t="inlineStr">
         <is>
-          <t>7310720A</t>
+          <t>7310720</t>
         </is>
       </c>
       <c r="B2799" s="23">
@@ -28383,7 +28383,7 @@
     <row r="2800" spans="1:2" s="0" outlineLevel="0">
       <c r="A2800" t="inlineStr">
         <is>
-          <t>7310723A</t>
+          <t>7310720A</t>
         </is>
       </c>
       <c r="B2800" s="23">
@@ -28393,7 +28393,7 @@
     <row r="2801" spans="1:2" s="0" outlineLevel="0">
       <c r="A2801" t="inlineStr">
         <is>
-          <t>7310723B</t>
+          <t>7310723A</t>
         </is>
       </c>
       <c r="B2801" s="23">
@@ -28403,7 +28403,7 @@
     <row r="2802" spans="1:2" s="0" outlineLevel="0">
       <c r="A2802" t="inlineStr">
         <is>
-          <t>7310724</t>
+          <t>7310723B</t>
         </is>
       </c>
       <c r="B2802" s="23">
@@ -28413,7 +28413,7 @@
     <row r="2803" spans="1:2" s="0" outlineLevel="0">
       <c r="A2803" t="inlineStr">
         <is>
-          <t>7310725</t>
+          <t>7310724</t>
         </is>
       </c>
       <c r="B2803" s="23">
@@ -28423,7 +28423,7 @@
     <row r="2804" spans="1:2" s="0" outlineLevel="0">
       <c r="A2804" t="inlineStr">
         <is>
-          <t>7310727A</t>
+          <t>7310725</t>
         </is>
       </c>
       <c r="B2804" s="23">
@@ -28433,7 +28433,7 @@
     <row r="2805" spans="1:2" s="0" outlineLevel="0">
       <c r="A2805" t="inlineStr">
         <is>
-          <t>7310727B</t>
+          <t>7310727A</t>
         </is>
       </c>
       <c r="B2805" s="23">
@@ -28443,7 +28443,7 @@
     <row r="2806" spans="1:2" s="0" outlineLevel="0">
       <c r="A2806" t="inlineStr">
         <is>
-          <t>7310728</t>
+          <t>7310727B</t>
         </is>
       </c>
       <c r="B2806" s="23">
@@ -28453,7 +28453,7 @@
     <row r="2807" spans="1:2" s="0" outlineLevel="0">
       <c r="A2807" t="inlineStr">
         <is>
-          <t>73107ONB</t>
+          <t>7310728</t>
         </is>
       </c>
       <c r="B2807" s="23">
@@ -28463,17 +28463,17 @@
     <row r="2808" spans="1:2" s="0" outlineLevel="0">
       <c r="A2808" t="inlineStr">
         <is>
-          <t>73109A0</t>
+          <t>73107ONB</t>
         </is>
       </c>
       <c r="B2808" s="23">
-        <v>73109</v>
+        <v>73107</v>
       </c>
     </row>
     <row r="2809" spans="1:2" s="0" outlineLevel="0">
       <c r="A2809" t="inlineStr">
         <is>
-          <t>73109B0</t>
+          <t>73109A0</t>
         </is>
       </c>
       <c r="B2809" s="23">
@@ -28483,7 +28483,7 @@
     <row r="2810" spans="1:2" s="0" outlineLevel="0">
       <c r="A2810" t="inlineStr">
         <is>
-          <t>73109C0</t>
+          <t>73109B0</t>
         </is>
       </c>
       <c r="B2810" s="23">
@@ -28493,7 +28493,7 @@
     <row r="2811" spans="1:2" s="0" outlineLevel="0">
       <c r="A2811" t="inlineStr">
         <is>
-          <t>73109D0</t>
+          <t>73109C0</t>
         </is>
       </c>
       <c r="B2811" s="23">
@@ -28503,7 +28503,7 @@
     <row r="2812" spans="1:2" s="0" outlineLevel="0">
       <c r="A2812" t="inlineStr">
         <is>
-          <t>73109E0</t>
+          <t>73109D0</t>
         </is>
       </c>
       <c r="B2812" s="23">
@@ -28513,7 +28513,7 @@
     <row r="2813" spans="1:2" s="0" outlineLevel="0">
       <c r="A2813" t="inlineStr">
         <is>
-          <t>73109F0</t>
+          <t>73109E0</t>
         </is>
       </c>
       <c r="B2813" s="23">
@@ -28523,7 +28523,7 @@
     <row r="2814" spans="1:2" s="0" outlineLevel="0">
       <c r="A2814" t="inlineStr">
         <is>
-          <t>73109ONB</t>
+          <t>73109F0</t>
         </is>
       </c>
       <c r="B2814" s="23">
@@ -28533,30 +28533,40 @@
     <row r="2815" spans="1:2" s="0" outlineLevel="0">
       <c r="A2815" t="inlineStr">
         <is>
-          <t>99991ONB</t>
+          <t>73109ONB</t>
         </is>
       </c>
       <c r="B2815" s="23">
-        <v>99991</v>
+        <v>73109</v>
       </c>
     </row>
     <row r="2816" spans="1:2" s="0" outlineLevel="0">
       <c r="A2816" t="inlineStr">
         <is>
-          <t>99992ONB</t>
+          <t>99991ONB</t>
         </is>
       </c>
       <c r="B2816" s="23">
-        <v>99992</v>
+        <v>99991</v>
       </c>
     </row>
     <row r="2817" spans="1:2" s="0" outlineLevel="0">
       <c r="A2817" t="inlineStr">
         <is>
+          <t>99992ONB</t>
+        </is>
+      </c>
+      <c r="B2817" s="23">
+        <v>99992</v>
+      </c>
+    </row>
+    <row r="2818" spans="1:2" s="0" outlineLevel="0">
+      <c r="A2818" t="inlineStr">
+        <is>
           <t>99999ONB</t>
         </is>
       </c>
-      <c r="B2817" s="23">
+      <c r="B2818" s="23">
         <v>99999</v>
       </c>
     </row>

</xml_diff>